<commit_message>
working on radius terms
</commit_message>
<xml_diff>
--- a/terms/radiusTerms.xlsx
+++ b/terms/radiusTerms.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanabalk/GitHub/futres/fovt/terms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D9455E-B057-1940-96A8-5E3813ECF875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408D84D4-B24A-3749-8F86-924066EB9201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16620" activeTab="1" xr2:uid="{DDED953A-1C75-5544-BDCF-AB53B1AEC9F2}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16620" xr2:uid="{DDED953A-1C75-5544-BDCF-AB53B1AEC9F2}"/>
   </bookViews>
   <sheets>
     <sheet name="trait" sheetId="1" r:id="rId1"/>
     <sheet name="axis" sheetId="3" r:id="rId2"/>
-    <sheet name="structures" sheetId="2" r:id="rId3"/>
+    <sheet name="circumference" sheetId="4" r:id="rId3"/>
+    <sheet name="structures" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
   <si>
     <t>FOVT STATUS</t>
   </si>
@@ -74,9 +75,6 @@
     <t>Ll</t>
   </si>
   <si>
-    <t>radius greatest length</t>
-  </si>
-  <si>
     <t>radius medial length</t>
   </si>
   <si>
@@ -135,6 +133,51 @@
   </si>
   <si>
     <t>Pattern name</t>
+  </si>
+  <si>
+    <t>radius length</t>
+  </si>
+  <si>
+    <t>in oba</t>
+  </si>
+  <si>
+    <t>proximal-distal</t>
+  </si>
+  <si>
+    <t>medialmost part of' some 'radius'</t>
+  </si>
+  <si>
+    <t>medial-lateral</t>
+  </si>
+  <si>
+    <t>diaphysis of radius</t>
+  </si>
+  <si>
+    <t>anterior-posterior</t>
+  </si>
+  <si>
+    <t>proximal epiphysis of radius</t>
+  </si>
+  <si>
+    <t>distal epiphysis of radius</t>
+  </si>
+  <si>
+    <t>humeral facet on radius</t>
+  </si>
+  <si>
+    <t>lateral side of' some radius</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>radio-carpal joint</t>
+  </si>
+  <si>
+    <t>lateral distal condyle breadth; radial notch</t>
+  </si>
+  <si>
+    <t>medial distal condyle breadth; ulnar notch</t>
   </si>
 </sst>
 </file>
@@ -177,9 +220,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DD2143-C7D2-8344-B8FF-72F5FC76860B}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,8 +573,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -540,16 +587,22 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
@@ -559,8 +612,11 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -568,7 +624,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -579,15 +635,18 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
@@ -598,7 +657,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
@@ -609,15 +668,18 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" t="s">
         <v>13</v>
@@ -628,7 +690,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
       </c>
       <c r="G12">
         <v>11</v>
@@ -636,15 +701,21 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
       </c>
       <c r="G13">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F14" t="s">
         <v>14</v>
@@ -652,18 +723,21 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" t="s">
         <v>29</v>
-      </c>
-      <c r="F15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -673,26 +747,164 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4206335-A915-8742-82F8-F72BF2C29968}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="67.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" t="s">
-        <v>35</v>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -701,6 +913,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5F7A78-C192-2F4F-902B-6214D68434A9}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD53E604-A5A6-0C41-A120-6C95F267A14E}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>